<commit_message>
add results for normalize-url
</commit_message>
<xml_diff>
--- a/casestudy/casestudy-results.xlsx
+++ b/casestudy/casestudy-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franktip/git/mutation-testing-data/casestudy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34136606-610D-6140-8C65-F8189B7E81E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F20883D-DA20-BB40-8E67-26AC2E9E0C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="1780" windowWidth="27640" windowHeight="16940" xr2:uid="{C52E8BFD-6907-DC4C-AC9A-6C7792B188BD}"/>
+    <workbookView xWindow="5360" yWindow="1780" windowWidth="33760" windowHeight="16940" xr2:uid="{C52E8BFD-6907-DC4C-AC9A-6C7792B188BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="154">
   <si>
     <t>application</t>
   </si>
@@ -1113,12 +1113,96 @@
   <si>
     <t>14  mutants, of which 8 produce the same failure as the original bug</t>
   </si>
+  <si>
+    <t>normalize-url</t>
+  </si>
+  <si>
+    <t>https://github.com/sindresorhus/normalize-url</t>
+  </si>
+  <si>
+    <t>191ad4b</t>
+  </si>
+  <si>
+    <t>if (options.removeTrailingSlash || urlObj.pathname === '/') {</t>
+  </si>
+  <si>
+    <t>if ((options.removeTrailingSlash || urlObj.pathname === '/') &amp;&amp; urlObj.hash === '') {</t>
+  </si>
+  <si>
+    <t>2 failed
+  removeTrailingSlash option
+  /Users/franktip/git/mutation-testing-data/casestudy/normalize-url-82/normalize-url/test.js:118
+   117:   t.is(normalizeUrl('http://sindresorhus.com/redirect/', options), 'http://sindresorhus.co…
+   118:   t.is(normalizeUrl('http://sindresorhus.com/#/', options), 'http://sindresorhus.com/#/'); 
+   119: });                                                                                        
+  Difference:
+  - 'http://sindresorhus.com/#'
+  + 'http://sindresorhus.com/#/'
+  Test.fn (test.js:118:4)
+  processEmit [as emit] (node_modules/nyc/node_modules/signal-exit/index.js:155:32)
+  processEmit [as emit] (node_modules/nyc/node_modules/signal-exit/index.js:155:32)
+  removeTrailingSlash and removeDirectoryIndex options)
+  /Users/franktip/git/mutation-testing-data/casestudy/normalize-url-82/normalize-url/test.js:155
+   154:   t.is(normalizeUrl('http://sindresorhus.com/path/index.html', options1), 'http://sindreso…
+   155:   t.is(normalizeUrl('http://sindresorhus.com/#/path/', options1), 'http://sindresorhus.com…
+   156:   t.is(normalizeUrl('http://sindresorhus.com/foo/#/bar/', options1), 'http://sindresorhus.…
+  Difference:
+  - 'http://sindresorhus.com/#/path'
+  + 'http://sindresorhus.com/#/path/'
+  Test.fn (test.js:155:4)
+  processEmit [as emit] (node_modules/nyc/node_modules/signal-exit/index.js:155:32)
+  processEmit [as emit] (node_modules/nyc/node_modules/signal-exit/index.js:155:32)</t>
+  </si>
+  <si>
+    <t>3  mutants, of which 1  produces the same failure as the original bug</t>
+  </si>
+  <si>
+    <t>3  mutants, of which 1  produces the same failures as the original bug</t>
+  </si>
+  <si>
+    <t>NOTE: disable "xo" in "npm run test" script; disable failing tests for invalid URLs</t>
+  </si>
+  <si>
+    <t>6078d91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1 failed
+  main
+  /Users/franktip/git/mutation-testing-data/casestudy/normalize-url-82/normalize-url/test.js:16
+   15:   t.is(m('http://www.sindresorhus.com'), 'http://sindresorhus.com');            
+   16:   t.is(m('www.com'), 'http://www.com');                                         
+   17:   t.is(m('http://www.www.sindresorhus.com'), 'http://www.www.sindresorhus.com');
+  Difference:
+  - 'http://com'
+  + 'http://www.com'
+  Test.fn (test.js:16:4)
+  processEmit [as emit] (node_modules/nyc/node_modules/signal-exit/index.js:155:32)
+  processEmit [as emit] (node_modules/nyc/node_modules/signal-exit/index.js:155:32)</t>
+  </si>
+  <si>
+    <t>if (opts.stripWWW) {</t>
+  </si>
+  <si>
+    <t>if (opts.stripWWW &amp;&amp; /^www\.([a-z\-\d]{2,63})\.([a-z\.]{2,5})$/.test(urlObj.hostname)) {</t>
+  </si>
+  <si>
+    <t>7  mutants, of which 1  produces the same failure as the original bug</t>
+  </si>
+  <si>
+    <t>7  mutants, of which 0  produce the same failure as the original bug</t>
+  </si>
+  <si>
+    <t>6  mutants, of which 2 produce the same failure as the original bug</t>
+  </si>
+  <si>
+    <t>8  mutants, of which 2 produce the same failure as the original bug</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1191,6 +1275,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1213,7 +1302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1248,56 +1337,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1640,11 +1726,11 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
@@ -1661,7 +1747,7 @@
     <col min="15" max="15" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1711,7 +1797,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="221" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="221">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1755,20 +1841,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:18" ht="77" customHeight="1">
+      <c r="A3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="27">
         <v>24</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="24" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="5">
@@ -1783,28 +1869,28 @@
       <c r="I3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="88" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+    <row r="4" spans="1:18" ht="88" customHeight="1">
+      <c r="A4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="5">
         <v>46</v>
       </c>
@@ -1817,13 +1903,13 @@
       <c r="I4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-    </row>
-    <row r="5" spans="1:18" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+    </row>
+    <row r="5" spans="1:18" ht="62" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
@@ -1867,7 +1953,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="89" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>42</v>
       </c>
@@ -1886,10 +1972,10 @@
       <c r="F6" s="5">
         <v>2069</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="14" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1911,7 +1997,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="161" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="161" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
@@ -1930,10 +2016,10 @@
       <c r="F7" s="5">
         <v>1884</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="15" t="s">
         <v>46</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1955,14 +2041,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="143" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="143" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>853</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -1971,13 +2057,13 @@
       <c r="E8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="13">
         <v>1008</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="16" t="s">
         <v>59</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1999,7 +2085,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="134" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="134" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>42</v>
       </c>
@@ -2009,7 +2095,7 @@
       <c r="C9" s="5">
         <v>59</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>63</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -2018,10 +2104,10 @@
       <c r="F9" s="5">
         <v>847</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="15" t="s">
         <v>65</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -2036,24 +2122,24 @@
       <c r="L9" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="M9" s="20" t="s">
+      <c r="M9" s="17" t="s">
         <v>69</v>
       </c>
       <c r="N9" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:18" ht="63" customHeight="1">
+      <c r="A10" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="27">
         <v>633</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2065,7 +2151,7 @@
       <c r="G10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="18" t="s">
         <v>75</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -2087,11 +2173,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12"/>
+    <row r="11" spans="1:18" ht="47" customHeight="1">
+      <c r="A11" s="26"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="5" t="s">
         <v>74</v>
       </c>
@@ -2101,7 +2187,7 @@
       <c r="G11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="19" t="s">
         <v>78</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -2123,17 +2209,17 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="144" customHeight="1">
       <c r="A12" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="5">
         <v>334</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="13" t="s">
         <v>81</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -2166,21 +2252,21 @@
       <c r="N12" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="O12" s="25" t="s">
+      <c r="O12" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="83" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="5">
         <v>223</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="13" t="s">
         <v>94</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -2217,17 +2303,17 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="289" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="289">
       <c r="A14" s="10" t="s">
         <v>102</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="5">
         <v>190</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="13" t="s">
         <v>104</v>
       </c>
       <c r="E14" s="10" t="s">
@@ -2236,10 +2322,10 @@
       <c r="F14" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="21" t="s">
         <v>108</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -2261,23 +2347,23 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="136" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:18" ht="136">
+      <c r="A15" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="24">
         <v>679</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="22">
         <v>107</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -2289,28 +2375,28 @@
       <c r="I15" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="L15" s="29" t="s">
+      <c r="L15" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="M15" s="29" t="s">
+      <c r="M15" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="N15" s="29" t="s">
+      <c r="N15" s="28" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+    <row r="16" spans="1:18" ht="108" customHeight="1">
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="5">
         <v>136</v>
       </c>
@@ -2323,23 +2409,23 @@
       <c r="I16" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-    </row>
-    <row r="17" spans="1:14" ht="323" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+    </row>
+    <row r="17" spans="1:15" ht="323">
+      <c r="A17" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="5">
         <v>291</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="13" t="s">
         <v>127</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -2357,78 +2443,166 @@
       <c r="I17" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="L17" s="29" t="s">
+      <c r="L17" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="M17" s="29" t="s">
+      <c r="M17" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="N17" s="29" t="s">
+      <c r="N17" s="28" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="14"/>
+    <row r="18" spans="1:15">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="16"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+    </row>
+    <row r="19" spans="1:15" ht="409.6">
+      <c r="A19" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="5">
+        <v>82</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="11">
+        <v>140</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="149" customHeight="1">
+      <c r="A20" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="5">
+        <v>38</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="5">
+        <v>103</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15">
       <c r="D32" s="4"/>
     </row>
   </sheetData>
@@ -2478,6 +2652,8 @@
     <hyperlink ref="B14" r:id="rId10" xr:uid="{85212475-E9DF-9346-B54D-00A6479F5031}"/>
     <hyperlink ref="B15" r:id="rId11" xr:uid="{7B51BD02-178C-1243-84F3-869E36370B44}"/>
     <hyperlink ref="B17" r:id="rId12" xr:uid="{D7C44975-8CD0-F54B-A507-870B5816BA89}"/>
+    <hyperlink ref="B19" r:id="rId13" xr:uid="{7D380E9C-453B-A64F-A27A-1EF0A86A1B49}"/>
+    <hyperlink ref="B20" r:id="rId14" xr:uid="{6685889E-162C-1147-8EC1-EA437BD2A95E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>